<commit_message>
updated repo with last versions of the files
</commit_message>
<xml_diff>
--- a/Diets by period.xlsx
+++ b/Diets by period.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="I-BCS" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="I-wo cereals" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="II-BCS" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="II-wo seaweed" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="III-BCS" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="III-wo greenhouses" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="I - OS" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="I - AS" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="II - OS" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="II - AS" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="III- OS" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="III - AS" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="26">
   <si>
     <t>g</t>
   </si>
@@ -27,74 +27,85 @@
     <t>Total:</t>
   </si>
   <si>
-    <t>Cattle (meat, mechanically separated)</t>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Wheat flour</t>
+  </si>
+  <si>
+    <t>Barley (pearled)</t>
+  </si>
+  <si>
+    <t>Canola oil</t>
+  </si>
+  <si>
+    <t>Rice (white)</t>
+  </si>
+  <si>
+    <t>Corn flour (whole-grain)</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Soy flour</t>
+  </si>
+  <si>
+    <t>Soybeans</t>
+  </si>
+  <si>
+    <t>Anchovy (raw)</t>
+  </si>
+  <si>
+    <t>Cattle (lean)</t>
+  </si>
+  <si>
+    <t>Cattle (organs)</t>
   </si>
   <si>
     <t>Milk (whole)</t>
   </si>
   <si>
-    <t>Rice</t>
-  </si>
-  <si>
-    <t>Potatoes</t>
-  </si>
-  <si>
-    <t>Barley</t>
-  </si>
-  <si>
-    <t>Anchovy</t>
-  </si>
-  <si>
-    <t>Canola oil</t>
-  </si>
-  <si>
-    <t>Soy flour</t>
-  </si>
-  <si>
-    <t>Cattle (organs)</t>
-  </si>
-  <si>
-    <t>Bread (whole-wheat)</t>
+    <t>Cattle (fat)</t>
   </si>
   <si>
     <t>Sugar (beets)</t>
   </si>
   <si>
+    <t>Wheat (hard red spring)</t>
+  </si>
+  <si>
+    <t>Rice (brown)</t>
+  </si>
+  <si>
     <t>Emi-tsunomata (dry)</t>
   </si>
   <si>
     <t>Laver (dry)</t>
   </si>
   <si>
-    <t>Wheat, hard red spring</t>
-  </si>
-  <si>
     <t>Lignocellulosic sugar</t>
   </si>
   <si>
-    <t>Corn</t>
-  </si>
-  <si>
-    <t>Kelp (dry)</t>
+    <t>Spirulina (dry)</t>
   </si>
   <si>
     <t>Wakame (dry)</t>
   </si>
   <si>
-    <t>Bacteria (methan)</t>
+    <t>Bacteria (methane)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -114,14 +125,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -373,7 +381,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1204.0</v>
+        <v>1417.0</v>
       </c>
       <c r="C2" s="1">
         <v>2100.0</v>
@@ -384,10 +392,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>36.2</v>
+        <v>344.8</v>
       </c>
       <c r="C3" s="1">
-        <v>100.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="4">
@@ -395,10 +403,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>245.9</v>
+        <v>68.7</v>
       </c>
       <c r="C4" s="1">
-        <v>150.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="5">
@@ -406,10 +414,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>54.8</v>
+        <v>24.4</v>
       </c>
       <c r="C5" s="1">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="6">
@@ -417,10 +425,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>459.8</v>
+        <v>19.2</v>
       </c>
       <c r="C6" s="1">
-        <v>400.0</v>
+        <v>170.0</v>
       </c>
     </row>
     <row r="7">
@@ -428,10 +436,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>56.5</v>
+        <v>115.4</v>
       </c>
       <c r="C7" s="1">
-        <v>200.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="8">
@@ -439,10 +447,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>152.7</v>
+        <v>27.7</v>
       </c>
       <c r="C8" s="1">
-        <v>200.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="9">
@@ -450,10 +458,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>39.6</v>
+        <v>104.2</v>
       </c>
       <c r="C9" s="1">
-        <v>350.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="10">
@@ -461,10 +469,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>69.1</v>
+        <v>46.1</v>
       </c>
       <c r="C10" s="1">
-        <v>300.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="11">
@@ -472,20 +480,53 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>35.8</v>
+        <v>116.3</v>
       </c>
       <c r="C11" s="1">
-        <v>50.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
-        <v>54.0</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1">
+        <v>76.3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>49.3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>178.8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>250.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>245.9</v>
+      </c>
+      <c r="C15" s="1">
         <v>150.0</v>
       </c>
     </row>
@@ -517,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1760.0</v>
+        <v>1555.0</v>
       </c>
       <c r="C2" s="1">
         <v>2100.0</v>
@@ -528,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>181.2</v>
+        <v>574.7</v>
       </c>
       <c r="C3" s="1">
         <v>500.0</v>
@@ -536,32 +577,32 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>409.8</v>
+        <v>114.5</v>
       </c>
       <c r="C4" s="1">
-        <v>250.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>747.1</v>
+        <v>221.7</v>
       </c>
       <c r="C5" s="1">
-        <v>650.0</v>
+        <v>450.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>190.8</v>
+        <v>36.8</v>
       </c>
       <c r="C6" s="1">
         <v>250.0</v>
@@ -569,24 +610,35 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>178.8</v>
+        <v>214.6</v>
       </c>
       <c r="C7" s="1">
-        <v>250.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>51.9</v>
+        <v>327.9</v>
       </c>
       <c r="C8" s="1">
         <v>200.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>64.9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>250.0</v>
       </c>
     </row>
   </sheetData>
@@ -617,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1444.0</v>
+        <v>1367.0</v>
       </c>
       <c r="C2" s="1">
         <v>2100.0</v>
@@ -628,21 +680,21 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>18.1</v>
+        <v>574.7</v>
       </c>
       <c r="C3" s="1">
-        <v>50.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>163.9</v>
+        <v>85.1</v>
       </c>
       <c r="C4" s="1">
-        <v>100.0</v>
+        <v>280.0</v>
       </c>
     </row>
     <row r="5">
@@ -650,10 +702,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>54.8</v>
+        <v>24.4</v>
       </c>
       <c r="C5" s="1">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="6">
@@ -661,87 +713,120 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>747.1</v>
+        <v>20.4</v>
       </c>
       <c r="C6" s="1">
-        <v>650.0</v>
+        <v>180.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
-        <v>57.9</v>
+        <v>81.3</v>
       </c>
       <c r="C7" s="1">
-        <v>150.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>23.8</v>
+        <v>51.8</v>
       </c>
       <c r="C8" s="1">
-        <v>50.0</v>
+        <v>225.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>190.8</v>
+        <v>29.1</v>
       </c>
       <c r="C9" s="1">
-        <v>250.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>22.6</v>
+        <v>76.3</v>
       </c>
       <c r="C10" s="1">
-        <v>200.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>57.6</v>
+        <v>73.9</v>
       </c>
       <c r="C11" s="1">
-        <v>250.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>71.5</v>
+        <v>16.2</v>
       </c>
       <c r="C12" s="1">
-        <v>100.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>36.0</v>
+        <v>57.2</v>
       </c>
       <c r="C13" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>204.9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>38.6</v>
+      </c>
+      <c r="C15" s="1">
         <v>100.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>33.3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>70.0</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1488.0</v>
+        <v>1338.0</v>
       </c>
       <c r="C2" s="1">
         <v>2100.0</v>
@@ -783,21 +868,21 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>18.1</v>
+        <v>574.7</v>
       </c>
       <c r="C3" s="1">
-        <v>50.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>245.9</v>
+        <v>85.1</v>
       </c>
       <c r="C4" s="1">
-        <v>150.0</v>
+        <v>280.0</v>
       </c>
     </row>
     <row r="5">
@@ -805,10 +890,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>54.8</v>
+        <v>24.4</v>
       </c>
       <c r="C5" s="1">
-        <v>200.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="6">
@@ -816,51 +901,51 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>747.1</v>
+        <v>20.4</v>
       </c>
       <c r="C6" s="1">
-        <v>650.0</v>
+        <v>180.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
-        <v>190.8</v>
+        <v>81.3</v>
       </c>
       <c r="C7" s="1">
-        <v>250.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>22.6</v>
+        <v>51.8</v>
       </c>
       <c r="C8" s="1">
-        <v>200.0</v>
+        <v>225.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>46.1</v>
+        <v>29.1</v>
       </c>
       <c r="C9" s="1">
-        <v>200.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>30.4</v>
+        <v>76.3</v>
       </c>
       <c r="C10" s="1">
         <v>100.0</v>
@@ -868,35 +953,57 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>71.5</v>
+        <v>73.9</v>
       </c>
       <c r="C11" s="1">
-        <v>100.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>25.0</v>
+        <v>16.2</v>
       </c>
       <c r="C12" s="1">
-        <v>100.0</v>
+        <v>110.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>36.0</v>
+        <v>57.2</v>
       </c>
       <c r="C13" s="1">
-        <v>100.0</v>
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>204.9</v>
+      </c>
+      <c r="C14" s="1">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>170.0</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>941.0</v>
+        <v>1232.0</v>
       </c>
       <c r="C2" s="1">
         <v>2100.0</v>
@@ -935,13 +1042,13 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>82.2</v>
+        <v>574.7</v>
       </c>
       <c r="C3" s="1">
-        <v>300.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="4">
@@ -949,32 +1056,32 @@
         <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>348.8</v>
+        <v>76.0</v>
       </c>
       <c r="C4" s="1">
-        <v>300.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>172.4</v>
+        <v>40.7</v>
       </c>
       <c r="C5" s="1">
-        <v>150.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>48.3</v>
+        <v>22.6</v>
       </c>
       <c r="C6" s="1">
-        <v>125.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="7">
@@ -982,87 +1089,120 @@
         <v>19</v>
       </c>
       <c r="B7" s="1">
-        <v>9.7</v>
+        <v>81.3</v>
       </c>
       <c r="C7" s="1">
-        <v>25.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>23.8</v>
+        <v>41.6</v>
       </c>
       <c r="C8" s="1">
-        <v>50.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>9.3</v>
+        <v>140.6</v>
       </c>
       <c r="C9" s="1">
-        <v>25.0</v>
+        <v>135.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>33.3</v>
+        <v>46.1</v>
       </c>
       <c r="C10" s="1">
-        <v>175.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>56.5</v>
+        <v>46.5</v>
       </c>
       <c r="C11" s="1">
-        <v>200.0</v>
+        <v>80.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>33.9</v>
+        <v>41.0</v>
       </c>
       <c r="C12" s="1">
-        <v>300.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
-        <v>69.1</v>
+        <v>17.2</v>
       </c>
       <c r="C13" s="1">
-        <v>300.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
-        <v>54.0</v>
+        <v>38.6</v>
       </c>
       <c r="C14" s="1">
-        <v>150.0</v>
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>38.0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>200.0</v>
       </c>
     </row>
   </sheetData>
@@ -1074,6 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1093,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1071.0</v>
+        <v>1121.0</v>
       </c>
       <c r="C2" s="1">
         <v>2100.0</v>
@@ -1101,115 +1242,140 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>689.7</v>
+        <v>574.7</v>
       </c>
       <c r="C3" s="1">
-        <v>600.0</v>
+        <v>500.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
-        <v>50.2</v>
+        <v>106.4</v>
       </c>
       <c r="C4" s="1">
-        <v>130.0</v>
+        <v>350.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>3.9</v>
+        <v>40.7</v>
       </c>
       <c r="C5" s="1">
-        <v>10.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>23.8</v>
+        <v>28.3</v>
       </c>
       <c r="C6" s="1">
-        <v>50.0</v>
+        <v>250.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>3.7</v>
+        <v>29.4</v>
       </c>
       <c r="C7" s="1">
-        <v>10.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>38.0</v>
+        <v>163.9</v>
       </c>
       <c r="C8" s="1">
-        <v>200.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
-        <v>70.6</v>
+        <v>17.2</v>
       </c>
       <c r="C9" s="1">
-        <v>250.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
-        <v>45.2</v>
+        <v>38.6</v>
       </c>
       <c r="C10" s="1">
-        <v>400.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1">
-        <v>37.5</v>
+        <v>23.8</v>
       </c>
       <c r="C11" s="1">
-        <v>150.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
-        <v>107.9</v>
+        <v>9.3</v>
       </c>
       <c r="C12" s="1">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1">
+        <v>57.0</v>
+      </c>
+      <c r="C13" s="1">
         <v>300.0</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1">
+        <v>31.3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>125.0</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>